<commit_message>
Added database patterns to programatic specifications
</commit_message>
<xml_diff>
--- a/docs/source/notes/COBRA_structure_fields.xlsx
+++ b/docs/source/notes/COBRA_structure_fields.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="151">
   <si>
     <t xml:space="preserve">Model Field</t>
   </si>
@@ -47,6 +47,9 @@
     <t xml:space="preserve">Default Value</t>
   </si>
   <si>
+    <t xml:space="preserve">DBPatterns</t>
+  </si>
+  <si>
     <t xml:space="preserve">S</t>
   </si>
   <si>
@@ -140,36 +143,54 @@
     <t xml:space="preserve">is</t>
   </si>
   <si>
+    <t xml:space="preserve">^HMDB\d{5}$</t>
+  </si>
+  <si>
     <t xml:space="preserve">metInChIString</t>
   </si>
   <si>
     <t xml:space="preserve">inchi</t>
   </si>
   <si>
+    <t xml:space="preserve">^InChI\=1S?\/[A-Za-z0-9]+(\+[0-9]+)?(\/[cnpqbtmsih][A-Za-z0-9\-\+\(\)\,\/]+)*$</t>
+  </si>
+  <si>
     <t xml:space="preserve">metKEGGID</t>
   </si>
   <si>
     <t xml:space="preserve">kegg.compound;kegg</t>
   </si>
   <si>
+    <t xml:space="preserve">^C\d+$</t>
+  </si>
+  <si>
     <t xml:space="preserve">metChEBIID</t>
   </si>
   <si>
     <t xml:space="preserve">chebi;obo.chebi</t>
   </si>
   <si>
+    <t xml:space="preserve">^CHEBI:\d+$</t>
+  </si>
+  <si>
     <t xml:space="preserve">metPubChemID</t>
   </si>
   <si>
     <t xml:space="preserve">pubchem.compound</t>
   </si>
   <si>
+    <t xml:space="preserve">^\d+$</t>
+  </si>
+  <si>
     <t xml:space="preserve">metMetaNetXID</t>
   </si>
   <si>
     <t xml:space="preserve">metnetx.chemical</t>
   </si>
   <si>
+    <t xml:space="preserve">^MNXM\d+$</t>
+  </si>
+  <si>
     <t xml:space="preserve">description</t>
   </si>
   <si>
@@ -230,6 +251,9 @@
     <t xml:space="preserve">ec-code</t>
   </si>
   <si>
+    <t xml:space="preserve">^\d+\.-\.-\.-|\d+\.\d+\.-\.-|\d+\.\d+\.\d+\.-|\d+\.\d+\.\d+\.(n)?\d+$</t>
+  </si>
+  <si>
     <t xml:space="preserve">rxnReferences</t>
   </si>
   <si>
@@ -243,6 +267,9 @@
   </si>
   <si>
     <t xml:space="preserve">kegg.reaction;kegg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^R\d+$</t>
   </si>
   <si>
     <t xml:space="preserve">subSystems</t>
@@ -562,22 +589,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H25" activeCellId="0" sqref="H25"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I:I"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.6224489795918"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="76.6734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -605,19 +634,22 @@
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>0</v>
@@ -625,16 +657,16 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>0</v>
@@ -642,33 +674,33 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>-1000</v>
@@ -676,16 +708,16 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>1000</v>
@@ -693,16 +725,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>0</v>
@@ -710,7 +742,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="n">
         <v>1</v>
@@ -719,7 +751,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>-1</v>
@@ -727,425 +759,446 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C14" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C15" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C16" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C17" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C18" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="G19" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C20" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C21" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C22" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C23" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C26" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C27" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C28" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="H29" s="0" t="n">
         <v>0</v>
@@ -1153,16 +1206,16 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C30" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H30" s="0" t="n">
         <v>0</v>
@@ -1170,199 +1223,208 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C31" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C32" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C33" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C34" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C35" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="I35" s="0" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C36" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="C37" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="C38" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C39" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C40" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1384,16 +1446,16 @@
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="I:I B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.8163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="176.301020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.2755102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="174.275510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1401,559 +1463,559 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed buildRxnGeneMat and updated dependent functions
</commit_message>
<xml_diff>
--- a/docs/source/notes/COBRA_structure_fields.xlsx
+++ b/docs/source/notes/COBRA_structure_fields.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Programatic Specification" sheetId="1" state="visible" r:id="rId2"/>
@@ -452,7 +452,7 @@
     <t xml:space="preserve">E.C. number for each reaction.</t>
   </si>
   <si>
-    <t xml:space="preserve">g x n</t>
+    <t xml:space="preserve">n x g </t>
   </si>
   <si>
     <t xml:space="preserve">Sparse or Full Matrix of Double or Boolean</t>
@@ -555,7 +555,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -570,6 +570,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -591,22 +595,21 @@
   </sheetPr>
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I:I"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="76.6734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.8673469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="13.2295918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1445,17 +1448,17 @@
   </sheetPr>
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="I:I B4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.2755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="174.275510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="172.382653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="13.2295918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1934,11 +1937,11 @@
         <v>142</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="4" t="s">
         <v>143</v>
       </c>
       <c r="C35" s="1" t="s">

</xml_diff>